<commit_message>
Pooh Points: normal 20260218
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-18.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-18.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -1171,14 +1171,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H9" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" t="n">
         <v>12</v>
-      </c>
-      <c r="I9" t="n">
-        <v>9</v>
       </c>
       <c r="J9" t="n">
         <v>5</v>
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>1</v>
@@ -1199,19 +1199,19 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="Q9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1527,19 +1527,19 @@
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -2155,41 +2155,41 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I21" t="n">
         <v>4</v>
       </c>
       <c r="J21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" t="n">
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2483,14 +2483,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -2505,25 +2505,25 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" t="n">
         <v>1</v>
       </c>
       <c r="P25" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U25" t="n">
         <v>0</v>
@@ -2632,68 +2632,68 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Aden Holloway</t>
+          <t>Keyshawn Hall</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ARK@ALA</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Final/2OT</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I27" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J27" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" t="n">
         <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q27" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R27" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="S27" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U27" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V27" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28">
@@ -2714,35 +2714,35 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Keyshawn Hall</t>
+          <t>Aden Holloway</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>ARK@ALA</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I28" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -2751,31 +2751,31 @@
         <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R28" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U28" t="n">
         <v>4</v>
       </c>
       <c r="V28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -2811,21 +2811,21 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H29" t="n">
+        <v>12</v>
+      </c>
+      <c r="I29" t="n">
+        <v>9</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" t="n">
         <v>7</v>
       </c>
-      <c r="I29" t="n">
-        <v>5</v>
-      </c>
-      <c r="J29" t="n">
-        <v>2</v>
-      </c>
-      <c r="K29" t="n">
-        <v>5</v>
-      </c>
       <c r="L29" t="n">
         <v>0</v>
       </c>
@@ -2839,25 +2839,25 @@
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="Q29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R29" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V29" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -2893,11 +2893,11 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I30" t="n">
         <v>3</v>
@@ -2921,19 +2921,19 @@
         <v>1</v>
       </c>
       <c r="P30" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q30" t="n">
         <v>1</v>
       </c>
       <c r="R30" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S30" t="n">
         <v>1</v>
       </c>
       <c r="T30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U30" t="n">
         <v>0</v>
@@ -3057,18 +3057,18 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
+        <v>7</v>
+      </c>
+      <c r="I32" t="n">
+        <v>2</v>
+      </c>
+      <c r="J32" t="n">
         <v>5</v>
       </c>
-      <c r="I32" t="n">
-        <v>2</v>
-      </c>
-      <c r="J32" t="n">
-        <v>3</v>
-      </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="P32" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q32" t="n">
         <v>1</v>
@@ -3795,14 +3795,14 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I41" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J41" t="n">
         <v>7</v>
@@ -3820,22 +3820,22 @@
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P41" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="Q41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R41" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T41" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U41" t="n">
         <v>3</v>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -4315,7 +4315,7 @@
         <v>2</v>
       </c>
       <c r="P47" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q47" t="n">
         <v>0</v>
@@ -5025,53 +5025,53 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I56" t="n">
+        <v>12</v>
+      </c>
+      <c r="J56" t="n">
+        <v>3</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>1</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>3</v>
+      </c>
+      <c r="P56" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>3</v>
+      </c>
+      <c r="R56" t="n">
+        <v>6</v>
+      </c>
+      <c r="S56" t="n">
+        <v>3</v>
+      </c>
+      <c r="T56" t="n">
+        <v>5</v>
+      </c>
+      <c r="U56" t="n">
+        <v>3</v>
+      </c>
+      <c r="V56" t="n">
         <v>4</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
-        <v>0</v>
-      </c>
-      <c r="O56" t="n">
-        <v>2</v>
-      </c>
-      <c r="P56" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>1</v>
-      </c>
-      <c r="R56" t="n">
-        <v>3</v>
-      </c>
-      <c r="S56" t="n">
-        <v>1</v>
-      </c>
-      <c r="T56" t="n">
-        <v>2</v>
-      </c>
-      <c r="U56" t="n">
-        <v>1</v>
-      </c>
-      <c r="V56" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -5681,17 +5681,17 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I64" t="n">
         <v>35</v>
       </c>
       <c r="J64" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K64" t="n">
         <v>2</v>
@@ -5709,19 +5709,19 @@
         <v>1</v>
       </c>
       <c r="P64" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="Q64" t="n">
         <v>13</v>
       </c>
       <c r="R64" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S64" t="n">
         <v>9</v>
       </c>
       <c r="T64" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U64" t="n">
         <v>0</v>
@@ -6404,38 +6404,38 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Tyler Tanner</t>
+          <t>Tahaad Pettiford</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H73" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I73" t="n">
         <v>11</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73" t="n">
         <v>0</v>
@@ -6447,7 +6447,7 @@
         <v>1</v>
       </c>
       <c r="P73" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="Q73" t="n">
         <v>4</v>
@@ -6456,16 +6456,16 @@
         <v>9</v>
       </c>
       <c r="S73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T73" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -6486,68 +6486,68 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Tahaad Pettiford</t>
+          <t>Tyler Tanner</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H74" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I74" t="n">
+        <v>13</v>
+      </c>
+      <c r="J74" t="n">
+        <v>2</v>
+      </c>
+      <c r="K74" t="n">
+        <v>3</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>2</v>
+      </c>
+      <c r="O74" t="n">
+        <v>1</v>
+      </c>
+      <c r="P74" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q74" t="n">
         <v>5</v>
       </c>
-      <c r="J74" t="n">
-        <v>2</v>
-      </c>
-      <c r="K74" t="n">
-        <v>3</v>
-      </c>
-      <c r="L74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M74" t="n">
-        <v>0</v>
-      </c>
-      <c r="N74" t="n">
-        <v>1</v>
-      </c>
-      <c r="O74" t="n">
-        <v>1</v>
-      </c>
-      <c r="P74" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q74" t="n">
-        <v>2</v>
-      </c>
       <c r="R74" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T74" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -6747,47 +6747,47 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H77" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I77" t="n">
         <v>10</v>
       </c>
       <c r="J77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K77" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L77" t="n">
         <v>1</v>
       </c>
       <c r="M77" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N77" t="n">
         <v>1</v>
       </c>
       <c r="O77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P77" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="Q77" t="n">
         <v>4</v>
       </c>
       <c r="R77" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S77" t="n">
         <v>2</v>
       </c>
       <c r="T77" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U77" t="n">
         <v>0</v>
@@ -6829,17 +6829,17 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I78" t="n">
         <v>6</v>
       </c>
       <c r="J78" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K78" t="n">
         <v>2</v>
@@ -6848,22 +6848,22 @@
         <v>2</v>
       </c>
       <c r="M78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N78" t="n">
         <v>1</v>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P78" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="Q78" t="n">
         <v>2</v>
       </c>
       <c r="R78" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -6911,11 +6911,11 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I79" t="n">
         <v>2</v>
@@ -6927,7 +6927,7 @@
         <v>1</v>
       </c>
       <c r="L79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" t="n">
         <v>0</v>
@@ -6936,16 +6936,16 @@
         <v>2</v>
       </c>
       <c r="O79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P79" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="Q79" t="n">
         <v>1</v>
       </c>
       <c r="R79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S79" t="n">
         <v>0</v>
@@ -10012,35 +10012,35 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Zach Clemence</t>
+          <t>T.O. Barrett</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>MISS@TA&amp;M</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H117" t="n">
         <v>13</v>
       </c>
       <c r="I117" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J117" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K117" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L117" t="n">
         <v>2</v>
@@ -10058,22 +10058,22 @@
         <v>24</v>
       </c>
       <c r="Q117" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R117" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="S117" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T117" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U117" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V117" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
@@ -10094,12 +10094,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Koren Johnson</t>
+          <t>Zach Clemence</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -10113,49 +10113,49 @@
         </is>
       </c>
       <c r="H118" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I118" t="n">
+        <v>14</v>
+      </c>
+      <c r="J118" t="n">
         <v>4</v>
       </c>
-      <c r="J118" t="n">
-        <v>2</v>
-      </c>
       <c r="K118" t="n">
+        <v>1</v>
+      </c>
+      <c r="L118" t="n">
+        <v>2</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" t="n">
+        <v>1</v>
+      </c>
+      <c r="O118" t="n">
+        <v>2</v>
+      </c>
+      <c r="P118" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q118" t="n">
         <v>6</v>
       </c>
-      <c r="L118" t="n">
-        <v>1</v>
-      </c>
-      <c r="M118" t="n">
-        <v>1</v>
-      </c>
-      <c r="N118" t="n">
-        <v>0</v>
-      </c>
-      <c r="O118" t="n">
-        <v>4</v>
-      </c>
-      <c r="P118" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q118" t="n">
-        <v>1</v>
-      </c>
       <c r="R118" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="S118" t="n">
         <v>0</v>
       </c>
       <c r="T118" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U118" t="n">
         <v>2</v>
       </c>
       <c r="V118" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
@@ -10176,68 +10176,68 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>T.O. Barrett</t>
+          <t>Koren Johnson</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>MISS@TA&amp;M</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H119" t="n">
         <v>10</v>
       </c>
       <c r="I119" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J119" t="n">
         <v>2</v>
       </c>
       <c r="K119" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O119" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P119" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="Q119" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R119" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="S119" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T119" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U119" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V119" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -10601,7 +10601,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -10626,7 +10626,7 @@
         <v>0</v>
       </c>
       <c r="O124" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P124" t="n">
         <v>10</v>
@@ -10832,56 +10832,56 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Achor Achor</t>
+          <t>Jayden Leverett</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H127" t="n">
+        <v>6</v>
+      </c>
+      <c r="I127" t="n">
+        <v>3</v>
+      </c>
+      <c r="J127" t="n">
+        <v>3</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" t="n">
+        <v>1</v>
+      </c>
+      <c r="M127" t="n">
+        <v>0</v>
+      </c>
+      <c r="N127" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="n">
+        <v>1</v>
+      </c>
+      <c r="P127" t="n">
         <v>5</v>
       </c>
-      <c r="I127" t="n">
-        <v>0</v>
-      </c>
-      <c r="J127" t="n">
-        <v>4</v>
-      </c>
-      <c r="K127" t="n">
-        <v>0</v>
-      </c>
-      <c r="L127" t="n">
-        <v>0</v>
-      </c>
-      <c r="M127" t="n">
-        <v>1</v>
-      </c>
-      <c r="N127" t="n">
-        <v>0</v>
-      </c>
-      <c r="O127" t="n">
-        <v>1</v>
-      </c>
-      <c r="P127" t="n">
-        <v>16</v>
-      </c>
       <c r="Q127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S127" t="n">
         <v>0</v>
@@ -10890,10 +10890,10 @@
         <v>0</v>
       </c>
       <c r="U127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V127" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -10914,35 +10914,35 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Amari Evans</t>
+          <t>Shawn Phillips Jr.</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>OU@TENN</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H128" t="n">
+        <v>6</v>
+      </c>
+      <c r="I128" t="n">
         <v>4</v>
       </c>
-      <c r="I128" t="n">
-        <v>0</v>
-      </c>
       <c r="J128" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L128" t="n">
         <v>1</v>
@@ -10951,19 +10951,19 @@
         <v>0</v>
       </c>
       <c r="N128" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O128" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P128" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q128" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R128" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S128" t="n">
         <v>0</v>
@@ -10975,7 +10975,7 @@
         <v>0</v>
       </c>
       <c r="V128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -10996,59 +10996,59 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Ja'Borri McGhee</t>
+          <t>Trent Burns</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H129" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I129" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J129" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L129" t="n">
         <v>0</v>
       </c>
       <c r="M129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O129" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P129" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="Q129" t="n">
         <v>1</v>
       </c>
       <c r="R129" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T129" t="n">
         <v>1</v>
@@ -11078,62 +11078,62 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Kai Rogers</t>
+          <t>Trent Pierce</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>OU@TENN</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H130" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I130" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M130" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O130" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P130" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="Q130" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R130" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S130" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T130" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U130" t="n">
         <v>0</v>
@@ -11160,56 +11160,56 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Malique Ewin</t>
+          <t>Amari Evans</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>ARK@ALA</t>
+          <t>OU@TENN</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Final/2OT</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H131" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I131" t="n">
         <v>0</v>
       </c>
       <c r="J131" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K131" t="n">
         <v>0</v>
       </c>
       <c r="L131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O131" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P131" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="Q131" t="n">
         <v>0</v>
       </c>
       <c r="R131" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S131" t="n">
         <v>0</v>
@@ -11242,38 +11242,38 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Trent Pierce</t>
+          <t>Filip Jović</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H132" t="n">
         <v>3</v>
       </c>
       <c r="I132" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K132" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M132" t="n">
         <v>0</v>
@@ -11285,25 +11285,25 @@
         <v>1</v>
       </c>
       <c r="P132" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="Q132" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R132" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T132" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U132" t="n">
         <v>0</v>
       </c>
       <c r="V132" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133">
@@ -11324,35 +11324,35 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>AK Okereke</t>
+          <t>Kai Rogers</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>OU@TENN</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H133" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I133" t="n">
         <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L133" t="n">
         <v>0</v>
@@ -11364,16 +11364,16 @@
         <v>1</v>
       </c>
       <c r="O133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P133" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q133" t="n">
         <v>0</v>
       </c>
       <c r="R133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S133" t="n">
         <v>0</v>
@@ -11406,56 +11406,56 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Filip Jović</t>
+          <t>Malique Ewin</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>ARK@ALA</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final/2OT</t>
         </is>
       </c>
       <c r="H134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I134" t="n">
         <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L134" t="n">
         <v>0</v>
       </c>
       <c r="M134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O134" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P134" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="Q134" t="n">
         <v>0</v>
       </c>
       <c r="R134" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S134" t="n">
         <v>0</v>
@@ -11467,7 +11467,7 @@
         <v>0</v>
       </c>
       <c r="V134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -11488,32 +11488,32 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Jacari Lane</t>
+          <t>Achor Achor</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>MISS@TA&amp;M</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H135" t="n">
         <v>2</v>
       </c>
       <c r="I135" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J135" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K135" t="n">
         <v>0</v>
@@ -11522,34 +11522,34 @@
         <v>0</v>
       </c>
       <c r="M135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N135" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P135" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="Q135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R135" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -11570,35 +11570,35 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Mike James</t>
+          <t>Jacari Lane</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>MISS@TA&amp;M</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H136" t="n">
         <v>2</v>
       </c>
       <c r="I136" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J136" t="n">
         <v>1</v>
       </c>
       <c r="K136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L136" t="n">
         <v>0</v>
@@ -11607,31 +11607,31 @@
         <v>0</v>
       </c>
       <c r="N136" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P136" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Q136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V136" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -11652,12 +11652,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Shawn Phillips Jr.</t>
+          <t>Mike James</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -11667,14 +11667,14 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H137" t="n">
         <v>2</v>
       </c>
       <c r="I137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
         <v>2</v>
@@ -11683,22 +11683,22 @@
         <v>1</v>
       </c>
       <c r="L137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M137" t="n">
         <v>0</v>
       </c>
       <c r="N137" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P137" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R137" t="n">
         <v>1</v>
@@ -11707,13 +11707,13 @@
         <v>0</v>
       </c>
       <c r="T137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
@@ -11734,68 +11734,68 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Ali Dibba</t>
+          <t>Sebastian Williams-Adams</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>MISS@TA&amp;M</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I138" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J138" t="n">
         <v>2</v>
       </c>
       <c r="K138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L138" t="n">
         <v>0</v>
       </c>
       <c r="M138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N138" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O138" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P138" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q138" t="n">
         <v>1</v>
       </c>
       <c r="R138" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S138" t="n">
         <v>0</v>
       </c>
       <c r="T138" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U138" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V138" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -11816,17 +11816,17 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Ethan Burg</t>
+          <t>Ali Dibba</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>OU@TENN</t>
+          <t>MISS@TA&amp;M</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -11838,10 +11838,10 @@
         <v>1</v>
       </c>
       <c r="I139" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J139" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K139" t="n">
         <v>0</v>
@@ -11853,31 +11853,31 @@
         <v>0</v>
       </c>
       <c r="N139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O139" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P139" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Q139" t="n">
         <v>1</v>
       </c>
       <c r="R139" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S139" t="n">
         <v>0</v>
       </c>
       <c r="T139" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U139" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V139" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140">
@@ -11898,29 +11898,29 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Jayden Leverett</t>
+          <t>Ethan Burg</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>OU@TENN</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H140" t="n">
         <v>1</v>
       </c>
       <c r="I140" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J140" t="n">
         <v>0</v>
@@ -11929,25 +11929,25 @@
         <v>0</v>
       </c>
       <c r="L140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M140" t="n">
         <v>0</v>
       </c>
       <c r="N140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P140" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Q140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S140" t="n">
         <v>0</v>
@@ -11980,22 +11980,22 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Pop Isaacs</t>
+          <t>Ja'Borri McGhee</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>MISS@TA&amp;M</t>
+          <t>AUB@MSST</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H141" t="n">
@@ -12005,7 +12005,7 @@
         <v>3</v>
       </c>
       <c r="J141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K141" t="n">
         <v>1</v>
@@ -12017,31 +12017,31 @@
         <v>0</v>
       </c>
       <c r="N141" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O141" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P141" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="Q141" t="n">
         <v>1</v>
       </c>
       <c r="R141" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V141" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -12062,50 +12062,50 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Sebastian Williams-Adams</t>
+          <t>Pop Isaacs</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>AUB@MSST</t>
+          <t>MISS@TA&amp;M</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H142" t="n">
         <v>1</v>
       </c>
       <c r="I142" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L142" t="n">
         <v>0</v>
       </c>
       <c r="M142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N142" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O142" t="n">
         <v>2</v>
       </c>
       <c r="P142" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Q142" t="n">
         <v>1</v>
@@ -12117,13 +12117,13 @@
         <v>0</v>
       </c>
       <c r="T142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V142" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
@@ -12159,7 +12159,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -12187,7 +12187,7 @@
         <v>0</v>
       </c>
       <c r="P143" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Q143" t="n">
         <v>0</v>
@@ -12226,22 +12226,22 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Trent Burns</t>
+          <t>Troy Henderson</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>VAN@MIZ</t>
+          <t>OU@TENN</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H144" t="n">
@@ -12251,7 +12251,7 @@
         <v>0</v>
       </c>
       <c r="J144" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K144" t="n">
         <v>0</v>
@@ -12269,13 +12269,13 @@
         <v>0</v>
       </c>
       <c r="P144" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q144" t="n">
         <v>0</v>
       </c>
       <c r="R144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S144" t="n">
         <v>0</v>
@@ -12308,17 +12308,17 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Troy Henderson</t>
+          <t>Zach Day</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>OU@TENN</t>
+          <t>MISS@TA&amp;M</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -12333,7 +12333,7 @@
         <v>0</v>
       </c>
       <c r="J145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K145" t="n">
         <v>0</v>
@@ -12345,13 +12345,13 @@
         <v>0</v>
       </c>
       <c r="N145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O145" t="n">
         <v>0</v>
       </c>
       <c r="P145" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q145" t="n">
         <v>0</v>
@@ -12390,26 +12390,26 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Zach Day</t>
+          <t>AK Okereke</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>MISS@TA&amp;M</t>
+          <t>VAN@MIZ</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I146" t="n">
         <v>0</v>
@@ -12424,22 +12424,22 @@
         <v>0</v>
       </c>
       <c r="M146" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O146" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P146" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="Q146" t="n">
         <v>0</v>
       </c>
       <c r="R146" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S146" t="n">
         <v>0</v>
@@ -12569,7 +12569,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Halftime</t>
+          <t>10:50 - 2nd Half</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -12979,7 +12979,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H153" t="n">
@@ -13004,10 +13004,10 @@
         <v>0</v>
       </c>
       <c r="O153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P153" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q153" t="n">
         <v>0</v>
@@ -13061,7 +13061,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -13071,7 +13071,7 @@
         <v>0</v>
       </c>
       <c r="J154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K154" t="n">
         <v>0</v>
@@ -13089,13 +13089,13 @@
         <v>2</v>
       </c>
       <c r="P154" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="Q154" t="n">
         <v>0</v>
       </c>
       <c r="R154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S154" t="n">
         <v>0</v>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>0:00 - 1st Half</t>
+          <t>12:15 - 2nd Half</t>
         </is>
       </c>
       <c r="H155" t="n">
@@ -13240,7 +13240,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -13253,7 +13253,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -13266,7 +13266,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -13292,7 +13292,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
@@ -13305,7 +13305,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>
@@ -13318,7 +13318,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
Pooh Points: final 20260218 -> PD14
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-18.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-18.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H43" t="n">
@@ -6337,7 +6337,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H72" t="n">
@@ -6829,7 +6829,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H78" t="n">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H115" t="n">
@@ -9945,7 +9945,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -10273,7 +10273,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -10437,7 +10437,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H122" t="n">
@@ -11257,7 +11257,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H132" t="n">
@@ -11421,7 +11421,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H134" t="n">
@@ -11585,7 +11585,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H136" t="n">
@@ -11913,7 +11913,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H140" t="n">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H142" t="n">
@@ -13007,7 +13007,7 @@
         <v>3</v>
       </c>
       <c r="P153" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q153" t="n">
         <v>0</v>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>0:06 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H155" t="n">

</xml_diff>